<commit_message>
Rewrite parseExcel, fix it and add extract new fields from excel files
</commit_message>
<xml_diff>
--- a/med/excel_files/Vrachi.xlsx
+++ b/med/excel_files/Vrachi.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dns\PycharmProjects\kursach3\medical-app-Artem\medical-app\med\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53C588-D36D-492F-AB34-C4A1FD7A7849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A49C1F1-8585-47F9-ABF3-1E886A6E667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$S$2:$S$76</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="442">
   <si>
     <t>id[pk]</t>
   </si>
@@ -1132,10 +1135,232 @@
     <t>frostman@yahoo.com</t>
   </si>
   <si>
+    <t>Клиники</t>
+  </si>
+  <si>
+    <t>1,5,9</t>
+  </si>
+  <si>
+    <t>2,4,6</t>
+  </si>
+  <si>
+    <t>1,6,11</t>
+  </si>
+  <si>
+    <t>1,8,10</t>
+  </si>
+  <si>
+    <t>2,7,9</t>
+  </si>
+  <si>
+    <t>2,13,14</t>
+  </si>
+  <si>
+    <t>3,5,9</t>
+  </si>
+  <si>
+    <t>4,7,9</t>
+  </si>
+  <si>
+    <t>11,12,13</t>
+  </si>
+  <si>
+    <t>14,16,19</t>
+  </si>
+  <si>
+    <t>1,7,17</t>
+  </si>
+  <si>
+    <t>1,16,18</t>
+  </si>
+  <si>
+    <t>4,9,15</t>
+  </si>
+  <si>
+    <t>15,17,18</t>
+  </si>
+  <si>
+    <t>7,11,12</t>
+  </si>
+  <si>
+    <t>6,8,9</t>
+  </si>
+  <si>
+    <t>5,7,19</t>
+  </si>
+  <si>
+    <t>13,14,17</t>
+  </si>
+  <si>
+    <t>1,8,9</t>
+  </si>
+  <si>
+    <t>1,10,13</t>
+  </si>
+  <si>
+    <t>5,15,17</t>
+  </si>
+  <si>
+    <t>6,17,19</t>
+  </si>
+  <si>
+    <t>13,14,15</t>
+  </si>
+  <si>
+    <t>12,17,18</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,6,13,14</t>
+  </si>
+  <si>
+    <t>4,8,9,10</t>
+  </si>
+  <si>
+    <t>7,8,9</t>
+  </si>
+  <si>
+    <t>1,13,15,19</t>
+  </si>
+  <si>
+    <t>2,7,9,10,11</t>
+  </si>
+  <si>
+    <t>3,4,5,6</t>
+  </si>
+  <si>
+    <t>17,18,19</t>
+  </si>
+  <si>
+    <t>3,5,7,9</t>
+  </si>
+  <si>
+    <t>2,8,10,11</t>
+  </si>
+  <si>
+    <t>13,14,19</t>
+  </si>
+  <si>
+    <t>2,5,6,7</t>
+  </si>
+  <si>
+    <t>5,9,13</t>
+  </si>
+  <si>
+    <t>7,8,9,11</t>
+  </si>
+  <si>
+    <t>2,7,8,15,17</t>
+  </si>
+  <si>
+    <t>2,6,7</t>
+  </si>
+  <si>
+    <t>5,8,9</t>
+  </si>
+  <si>
+    <t>4,6,10</t>
+  </si>
+  <si>
+    <t>15,16,19</t>
+  </si>
+  <si>
+    <t>5,8,9,17</t>
+  </si>
+  <si>
+    <t>2,5,15</t>
+  </si>
+  <si>
+    <t>3,4,8,11</t>
+  </si>
+  <si>
+    <t>4,7,8,9</t>
+  </si>
+  <si>
+    <t>6,16,17</t>
+  </si>
+  <si>
+    <t>1,3,7,9,14</t>
+  </si>
+  <si>
+    <t>3,8,9,18</t>
+  </si>
+  <si>
+    <t>1,6,7</t>
+  </si>
+  <si>
+    <t>3,6,7,8</t>
+  </si>
+  <si>
+    <t>2,4,14,15</t>
+  </si>
+  <si>
+    <t>1,11,19</t>
+  </si>
+  <si>
+    <t>3,6,9,11</t>
+  </si>
+  <si>
+    <t>4,5,7</t>
+  </si>
+  <si>
+    <t>4,9,11,14</t>
+  </si>
+  <si>
+    <t>13,15,17,19</t>
+  </si>
+  <si>
+    <t>4,9,11</t>
+  </si>
+  <si>
+    <t>3,4,6</t>
+  </si>
+  <si>
+    <t>7,13,14,16</t>
+  </si>
+  <si>
+    <t>6,9,11,17</t>
+  </si>
+  <si>
+    <t>13,14,15,16</t>
+  </si>
+  <si>
+    <t>2,6,8,13</t>
+  </si>
+  <si>
+    <t>1,7,9,15</t>
+  </si>
+  <si>
+    <t>2,8,9,13</t>
+  </si>
+  <si>
+    <t>2,7,13</t>
+  </si>
+  <si>
+    <t>3,7,9</t>
+  </si>
+  <si>
+    <t>4,9,10</t>
+  </si>
+  <si>
+    <t>Срок действия</t>
+  </si>
+  <si>
+    <t>Стаж</t>
+  </si>
+  <si>
+    <t>Номер медицинской лицензии</t>
+  </si>
+  <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
     <t>Пн</t>
-  </si>
-  <si>
-    <t>Фамилия</t>
   </si>
 </sst>
 </file>
@@ -1178,11 +1403,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1191,9 +1417,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1506,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4553112-A26D-C14D-AED8-4119DE26C473}">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,9 +1761,12 @@
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
     <col min="12" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="27.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="27" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>367</v>
+        <v>440</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1546,7 +1783,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>366</v>
+        <v>441</v>
       </c>
       <c r="G1" t="s">
         <v>196</v>
@@ -1572,8 +1809,20 @@
       <c r="N1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>366</v>
+      </c>
+      <c r="P1" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>437</v>
+      </c>
+      <c r="R1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1604,11 +1853,24 @@
       <c r="M2" t="s">
         <v>214</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="6" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>367</v>
+      </c>
+      <c r="P2" s="4">
+        <v>11822484</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>45225</v>
+      </c>
+      <c r="R2" s="1">
+        <v>13</v>
+      </c>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1642,8 +1904,21 @@
       <c r="N3" s="3" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>368</v>
+      </c>
+      <c r="P3" s="4">
+        <v>12055294</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>45715</v>
+      </c>
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1680,8 +1955,21 @@
       <c r="N4" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>369</v>
+      </c>
+      <c r="P4" s="4">
+        <v>12254657</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>44970</v>
+      </c>
+      <c r="R4" s="1">
+        <v>22</v>
+      </c>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1721,8 +2009,21 @@
       <c r="N5" s="3" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>370</v>
+      </c>
+      <c r="P5" s="4">
+        <v>16297862</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>45694</v>
+      </c>
+      <c r="R5" s="1">
+        <v>3</v>
+      </c>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1759,8 +2060,21 @@
       <c r="N6" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>371</v>
+      </c>
+      <c r="P6" s="4">
+        <v>17322873</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>46063</v>
+      </c>
+      <c r="R6" s="1">
+        <v>24</v>
+      </c>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1797,8 +2111,21 @@
       <c r="N7" s="3" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>372</v>
+      </c>
+      <c r="P7" s="4">
+        <v>17795222</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>46014</v>
+      </c>
+      <c r="R7" s="1">
+        <v>4</v>
+      </c>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1832,11 +2159,24 @@
       <c r="M8" t="s">
         <v>220</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="6" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>373</v>
+      </c>
+      <c r="P8" s="4">
+        <v>18172535</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>45762</v>
+      </c>
+      <c r="R8" s="1">
+        <v>30</v>
+      </c>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1870,8 +2210,21 @@
       <c r="N9" s="3" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>374</v>
+      </c>
+      <c r="P9" s="4">
+        <v>18284934</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>45975</v>
+      </c>
+      <c r="R9" s="1">
+        <v>5</v>
+      </c>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1908,8 +2261,21 @@
       <c r="N10" s="3" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>375</v>
+      </c>
+      <c r="P10" s="4">
+        <v>18371905</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>45544</v>
+      </c>
+      <c r="R10" s="1">
+        <v>35</v>
+      </c>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1946,8 +2312,21 @@
       <c r="N11" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>376</v>
+      </c>
+      <c r="P11" s="4">
+        <v>18595168</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>46174</v>
+      </c>
+      <c r="R11" s="1">
+        <v>6</v>
+      </c>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1984,8 +2363,21 @@
       <c r="N12" s="3" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>377</v>
+      </c>
+      <c r="P12" s="4">
+        <v>19128191</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>45938</v>
+      </c>
+      <c r="R12" s="1">
+        <v>31</v>
+      </c>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2022,8 +2414,21 @@
       <c r="N13" s="3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>378</v>
+      </c>
+      <c r="P13" s="4">
+        <v>20802616</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>45023</v>
+      </c>
+      <c r="R13" s="1">
+        <v>7</v>
+      </c>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2057,8 +2462,21 @@
       <c r="N14" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>379</v>
+      </c>
+      <c r="P14" s="4">
+        <v>21245770</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>45306</v>
+      </c>
+      <c r="R14" s="1">
+        <v>30</v>
+      </c>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2095,8 +2513,21 @@
       <c r="N15" s="3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>380</v>
+      </c>
+      <c r="P15" s="4">
+        <v>22566047</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>45994</v>
+      </c>
+      <c r="R15" s="1">
+        <v>8</v>
+      </c>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2133,8 +2564,21 @@
       <c r="N16" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>381</v>
+      </c>
+      <c r="P16" s="4">
+        <v>22654786</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>45768</v>
+      </c>
+      <c r="R16" s="1">
+        <v>25</v>
+      </c>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2171,8 +2615,21 @@
       <c r="N17" s="3" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>382</v>
+      </c>
+      <c r="P17" s="4">
+        <v>25162782</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>45128</v>
+      </c>
+      <c r="R17" s="1">
+        <v>9</v>
+      </c>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2209,8 +2666,21 @@
       <c r="N18" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>383</v>
+      </c>
+      <c r="P18" s="4">
+        <v>28807723</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>46183</v>
+      </c>
+      <c r="R18" s="1">
+        <v>23</v>
+      </c>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2244,8 +2714,21 @@
       <c r="N19" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>384</v>
+      </c>
+      <c r="P19" s="4">
+        <v>30063649</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>45509</v>
+      </c>
+      <c r="R19" s="1">
+        <v>10</v>
+      </c>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2282,8 +2765,21 @@
       <c r="N20" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>371</v>
+      </c>
+      <c r="P20" s="4">
+        <v>31027949</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>46001</v>
+      </c>
+      <c r="R20" s="1">
+        <v>44</v>
+      </c>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2320,8 +2816,21 @@
       <c r="N21" s="3" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>385</v>
+      </c>
+      <c r="P21" s="4">
+        <v>31789180</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>45462</v>
+      </c>
+      <c r="R21" s="1">
+        <v>11</v>
+      </c>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2358,8 +2867,21 @@
       <c r="N22" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>386</v>
+      </c>
+      <c r="P22" s="4">
+        <v>32148849</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>44980</v>
+      </c>
+      <c r="R22" s="1">
+        <v>30</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2396,8 +2918,21 @@
       <c r="N23" s="3" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>387</v>
+      </c>
+      <c r="P23" s="4">
+        <v>33498667</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>44896</v>
+      </c>
+      <c r="R23" s="1">
+        <v>12</v>
+      </c>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2434,8 +2969,21 @@
       <c r="N24" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>388</v>
+      </c>
+      <c r="P24" s="4">
+        <v>33934540</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>46175</v>
+      </c>
+      <c r="R24" s="1">
+        <v>6</v>
+      </c>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2472,8 +3020,21 @@
       <c r="N25" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>389</v>
+      </c>
+      <c r="P25" s="4">
+        <v>34264282</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>45071</v>
+      </c>
+      <c r="R25" s="1">
+        <v>13</v>
+      </c>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2510,8 +3071,21 @@
       <c r="N26" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>390</v>
+      </c>
+      <c r="P26" s="4">
+        <v>37014292</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>45147</v>
+      </c>
+      <c r="R26" s="1">
+        <v>37</v>
+      </c>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2548,8 +3122,21 @@
       <c r="N27" s="3" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>391</v>
+      </c>
+      <c r="P27" s="4">
+        <v>37627822</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>44855</v>
+      </c>
+      <c r="R27" s="1">
+        <v>14</v>
+      </c>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2589,8 +3176,21 @@
       <c r="N28" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>392</v>
+      </c>
+      <c r="P28" s="4">
+        <v>37833405</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>45313</v>
+      </c>
+      <c r="R28" s="1">
+        <v>17</v>
+      </c>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2627,8 +3227,21 @@
       <c r="N29" s="3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>393</v>
+      </c>
+      <c r="P29" s="4">
+        <v>37974605</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>45818</v>
+      </c>
+      <c r="R29" s="1">
+        <v>15</v>
+      </c>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2668,8 +3281,21 @@
       <c r="N30" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>430</v>
+      </c>
+      <c r="P30" s="4">
+        <v>39745681</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>45562</v>
+      </c>
+      <c r="R30" s="1">
+        <v>44</v>
+      </c>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2706,8 +3332,21 @@
       <c r="N31" s="3" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>394</v>
+      </c>
+      <c r="P31" s="4">
+        <v>40836014</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>45831</v>
+      </c>
+      <c r="R31" s="1">
+        <v>16</v>
+      </c>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2744,8 +3383,21 @@
       <c r="N32" s="3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>395</v>
+      </c>
+      <c r="P32" s="4">
+        <v>41950672</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>45492</v>
+      </c>
+      <c r="R32" s="1">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2782,8 +3434,21 @@
       <c r="N33" s="3" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>396</v>
+      </c>
+      <c r="P33" s="4">
+        <v>41957130</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>45000</v>
+      </c>
+      <c r="R33" s="1">
+        <v>17</v>
+      </c>
+      <c r="S33" s="1"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2820,8 +3485,21 @@
       <c r="N34" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>397</v>
+      </c>
+      <c r="P34" s="4">
+        <v>43463966</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>45134</v>
+      </c>
+      <c r="R34" s="1">
+        <v>43</v>
+      </c>
+      <c r="S34" s="1"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2858,8 +3536,21 @@
       <c r="N35" s="3" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>398</v>
+      </c>
+      <c r="P35" s="4">
+        <v>46634986</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>45797</v>
+      </c>
+      <c r="R35" s="1">
+        <v>18</v>
+      </c>
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2896,8 +3587,21 @@
       <c r="N36" s="3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>431</v>
+      </c>
+      <c r="P36" s="4">
+        <v>48448435</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>44847</v>
+      </c>
+      <c r="R36" s="1">
+        <v>48</v>
+      </c>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2931,8 +3635,21 @@
       <c r="N37" s="3" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>399</v>
+      </c>
+      <c r="P37" s="4">
+        <v>48699825</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>45239</v>
+      </c>
+      <c r="R37" s="1">
+        <v>19</v>
+      </c>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2972,8 +3689,21 @@
       <c r="N38" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
+        <v>400</v>
+      </c>
+      <c r="P38" s="4">
+        <v>50604707</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>45623</v>
+      </c>
+      <c r="R38" s="1">
+        <v>9</v>
+      </c>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3010,8 +3740,21 @@
       <c r="N39" s="3" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>400</v>
+      </c>
+      <c r="P39" s="4">
+        <v>50710108</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>45939</v>
+      </c>
+      <c r="R39" s="1">
+        <v>20</v>
+      </c>
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3048,8 +3791,21 @@
       <c r="N40" s="3" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>401</v>
+      </c>
+      <c r="P40" s="4">
+        <v>51280550</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>45448</v>
+      </c>
+      <c r="R40" s="1">
+        <v>29</v>
+      </c>
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3086,8 +3842,21 @@
       <c r="N41" s="3" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>402</v>
+      </c>
+      <c r="P41" s="4">
+        <v>52941154</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>45251</v>
+      </c>
+      <c r="R41" s="1">
+        <v>21</v>
+      </c>
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3124,8 +3893,21 @@
       <c r="N42" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>432</v>
+      </c>
+      <c r="P42" s="4">
+        <v>54446070</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>44995</v>
+      </c>
+      <c r="R42" s="1">
+        <v>50</v>
+      </c>
+      <c r="S42" s="1"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3162,8 +3944,21 @@
       <c r="N43" s="3" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>403</v>
+      </c>
+      <c r="P43" s="4">
+        <v>54823939</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>46010</v>
+      </c>
+      <c r="R43" s="1">
+        <v>22</v>
+      </c>
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3200,8 +3995,21 @@
       <c r="N44" s="3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" t="s">
+        <v>385</v>
+      </c>
+      <c r="P44" s="4">
+        <v>57379100</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>45828</v>
+      </c>
+      <c r="R44" s="1">
+        <v>1</v>
+      </c>
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3238,8 +4046,21 @@
       <c r="N45" s="3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" t="s">
+        <v>404</v>
+      </c>
+      <c r="P45" s="4">
+        <v>59092522</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>45288</v>
+      </c>
+      <c r="R45" s="1">
+        <v>23</v>
+      </c>
+      <c r="S45" s="1"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3273,8 +4094,21 @@
       <c r="N46" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>433</v>
+      </c>
+      <c r="P46" s="4">
+        <v>59382119</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>45111</v>
+      </c>
+      <c r="R46" s="1">
+        <v>20</v>
+      </c>
+      <c r="S46" s="1"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3308,8 +4142,21 @@
       <c r="N47" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>405</v>
+      </c>
+      <c r="P47" s="4">
+        <v>61826190</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>46099</v>
+      </c>
+      <c r="R47" s="1">
+        <v>24</v>
+      </c>
+      <c r="S47" s="1"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3343,8 +4190,21 @@
       <c r="N48" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>434</v>
+      </c>
+      <c r="P48" s="4">
+        <v>62122928</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>45520</v>
+      </c>
+      <c r="R48" s="1">
+        <v>17</v>
+      </c>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3381,8 +4241,21 @@
       <c r="N49" s="3" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>406</v>
+      </c>
+      <c r="P49" s="4">
+        <v>62357323</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>45281</v>
+      </c>
+      <c r="R49" s="1">
+        <v>25</v>
+      </c>
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3419,8 +4292,21 @@
       <c r="N50" s="3" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>435</v>
+      </c>
+      <c r="P50" s="4">
+        <v>65276201</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>45210</v>
+      </c>
+      <c r="R50" s="1">
+        <v>5</v>
+      </c>
+      <c r="S50" s="1"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3457,8 +4343,21 @@
       <c r="N51" s="3" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>385</v>
+      </c>
+      <c r="P51" s="4">
+        <v>65700118</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>45209</v>
+      </c>
+      <c r="R51" s="1">
+        <v>26</v>
+      </c>
+      <c r="S51" s="1"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3498,8 +4397,21 @@
       <c r="N52" s="3" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" t="s">
+        <v>407</v>
+      </c>
+      <c r="P52" s="4">
+        <v>65941581</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>46007</v>
+      </c>
+      <c r="R52" s="1">
+        <v>42</v>
+      </c>
+      <c r="S52" s="1"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3536,8 +4448,21 @@
       <c r="N53" s="3" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" t="s">
+        <v>408</v>
+      </c>
+      <c r="P53" s="4">
+        <v>66277993</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>45890</v>
+      </c>
+      <c r="R53" s="1">
+        <v>27</v>
+      </c>
+      <c r="S53" s="1"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3574,8 +4499,21 @@
       <c r="N54" s="3" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" t="s">
+        <v>409</v>
+      </c>
+      <c r="P54" s="4">
+        <v>66997059</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>45519</v>
+      </c>
+      <c r="R54" s="1">
+        <v>3</v>
+      </c>
+      <c r="S54" s="1"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3612,8 +4550,21 @@
       <c r="N55" s="3" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" t="s">
+        <v>436</v>
+      </c>
+      <c r="P55" s="4">
+        <v>68449437</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>45971</v>
+      </c>
+      <c r="R55" s="1">
+        <v>28</v>
+      </c>
+      <c r="S55" s="1"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3650,8 +4601,21 @@
       <c r="N56" s="3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>410</v>
+      </c>
+      <c r="P56" s="4">
+        <v>70006969</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>46041</v>
+      </c>
+      <c r="R56" s="1">
+        <v>17</v>
+      </c>
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3688,8 +4652,21 @@
       <c r="N57" s="3" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>411</v>
+      </c>
+      <c r="P57" s="4">
+        <v>70380990</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>45926</v>
+      </c>
+      <c r="R57" s="1">
+        <v>29</v>
+      </c>
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3726,8 +4703,21 @@
       <c r="N58" s="3" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" t="s">
+        <v>412</v>
+      </c>
+      <c r="P58" s="4">
+        <v>70598632</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>45706</v>
+      </c>
+      <c r="R58" s="1">
+        <v>5</v>
+      </c>
+      <c r="S58" s="1"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3767,8 +4757,21 @@
       <c r="N59" s="3" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>413</v>
+      </c>
+      <c r="P59" s="4">
+        <v>71377994</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>44867</v>
+      </c>
+      <c r="R59" s="1">
+        <v>30</v>
+      </c>
+      <c r="S59" s="1"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3805,8 +4808,21 @@
       <c r="N60" s="3" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>414</v>
+      </c>
+      <c r="P60" s="4">
+        <v>73457641</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>46022</v>
+      </c>
+      <c r="R60" s="1">
+        <v>3</v>
+      </c>
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3843,8 +4859,21 @@
       <c r="N61" s="3" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>415</v>
+      </c>
+      <c r="P61" s="4">
+        <v>75512282</v>
+      </c>
+      <c r="Q61" s="5">
+        <v>45861</v>
+      </c>
+      <c r="R61" s="1">
+        <v>31</v>
+      </c>
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3881,8 +4910,21 @@
       <c r="N62" s="3" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>417</v>
+      </c>
+      <c r="P62" s="4">
+        <v>79485523</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>46015</v>
+      </c>
+      <c r="R62" s="1">
+        <v>8</v>
+      </c>
+      <c r="S62" s="1"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3919,8 +4961,21 @@
       <c r="N63" s="3" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>416</v>
+      </c>
+      <c r="P63" s="4">
+        <v>81509908</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>45530</v>
+      </c>
+      <c r="R63" s="1">
+        <v>32</v>
+      </c>
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3957,8 +5012,21 @@
       <c r="N64" s="3" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" t="s">
+        <v>418</v>
+      </c>
+      <c r="P64" s="4">
+        <v>83947540</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>44945</v>
+      </c>
+      <c r="R64" s="1">
+        <v>40</v>
+      </c>
+      <c r="S64" s="1"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3992,8 +5060,21 @@
       <c r="N65" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" t="s">
+        <v>419</v>
+      </c>
+      <c r="P65" s="4">
+        <v>84107774</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>44859</v>
+      </c>
+      <c r="R65" s="1">
+        <v>33</v>
+      </c>
+      <c r="S65" s="1"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4030,8 +5111,21 @@
       <c r="N66" s="3" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66" t="s">
+        <v>420</v>
+      </c>
+      <c r="P66" s="4">
+        <v>84291047</v>
+      </c>
+      <c r="Q66" s="5">
+        <v>45084</v>
+      </c>
+      <c r="R66" s="1">
+        <v>8</v>
+      </c>
+      <c r="S66" s="1"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4065,8 +5159,21 @@
       <c r="N67" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67" t="s">
+        <v>421</v>
+      </c>
+      <c r="P67" s="4">
+        <v>85807361</v>
+      </c>
+      <c r="Q67" s="5">
+        <v>44998</v>
+      </c>
+      <c r="R67" s="1">
+        <v>34</v>
+      </c>
+      <c r="S67" s="1"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4103,8 +5210,21 @@
       <c r="N68" s="3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" t="s">
+        <v>422</v>
+      </c>
+      <c r="P68" s="4">
+        <v>87972805</v>
+      </c>
+      <c r="Q68" s="5">
+        <v>46147</v>
+      </c>
+      <c r="R68" s="1">
+        <v>9</v>
+      </c>
+      <c r="S68" s="1"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4141,8 +5261,21 @@
       <c r="N69" s="3" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69" t="s">
+        <v>423</v>
+      </c>
+      <c r="P69" s="4">
+        <v>88897500</v>
+      </c>
+      <c r="Q69" s="5">
+        <v>45761</v>
+      </c>
+      <c r="R69" s="1">
+        <v>35</v>
+      </c>
+      <c r="S69" s="1"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4179,8 +5312,21 @@
       <c r="N70" s="3" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" t="s">
+        <v>371</v>
+      </c>
+      <c r="P70" s="4">
+        <v>89052173</v>
+      </c>
+      <c r="Q70" s="5">
+        <v>44839</v>
+      </c>
+      <c r="R70" s="1">
+        <v>31</v>
+      </c>
+      <c r="S70" s="1"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4217,8 +5363,21 @@
       <c r="N71" s="3" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71" t="s">
+        <v>424</v>
+      </c>
+      <c r="P71" s="4">
+        <v>90551996</v>
+      </c>
+      <c r="Q71" s="5">
+        <v>45631</v>
+      </c>
+      <c r="R71" s="1">
+        <v>36</v>
+      </c>
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4255,8 +5414,21 @@
       <c r="N72" s="3" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72" t="s">
+        <v>425</v>
+      </c>
+      <c r="P72" s="4">
+        <v>93280059</v>
+      </c>
+      <c r="Q72" s="5">
+        <v>44816</v>
+      </c>
+      <c r="R72" s="1">
+        <v>28</v>
+      </c>
+      <c r="S72" s="1"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4293,8 +5465,21 @@
       <c r="N73" s="3" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" t="s">
+        <v>426</v>
+      </c>
+      <c r="P73" s="4">
+        <v>93724153</v>
+      </c>
+      <c r="Q73" s="5">
+        <v>45775</v>
+      </c>
+      <c r="R73" s="1">
+        <v>37</v>
+      </c>
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4328,8 +5513,21 @@
       <c r="N74" s="3" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" t="s">
+        <v>427</v>
+      </c>
+      <c r="P74" s="4">
+        <v>94005496</v>
+      </c>
+      <c r="Q74" s="5">
+        <v>46169</v>
+      </c>
+      <c r="R74" s="1">
+        <v>37</v>
+      </c>
+      <c r="S74" s="1"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4366,8 +5564,21 @@
       <c r="N75" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" t="s">
+        <v>428</v>
+      </c>
+      <c r="P75" s="4">
+        <v>96425416</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>45740</v>
+      </c>
+      <c r="R75" s="1">
+        <v>38</v>
+      </c>
+      <c r="S75" s="1"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4404,25 +5615,141 @@
       <c r="N76" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" t="s">
+        <v>429</v>
+      </c>
+      <c r="P76" s="4">
+        <v>99375666</v>
+      </c>
+      <c r="Q76" s="5">
+        <v>45572</v>
+      </c>
+      <c r="R76" s="1">
+        <v>43</v>
+      </c>
+      <c r="S76" s="1"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="N77" s="3"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P77" s="4"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="N78" s="3"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P78" s="4"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="N79" s="3"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P79" s="4"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="N80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P80" s="4"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P82" s="4"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P83" s="4"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P84" s="4"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P85" s="4"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P86" s="4"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q96" s="1"/>
+    </row>
+    <row r="97" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q97" s="1"/>
+    </row>
+    <row r="98" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q98" s="1"/>
+    </row>
+    <row r="99" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q99" s="1"/>
+    </row>
+    <row r="100" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q100" s="1"/>
+    </row>
+    <row r="101" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q101" s="1"/>
+    </row>
+    <row r="102" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q102" s="1"/>
+    </row>
+    <row r="103" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q103" s="1"/>
+    </row>
+    <row r="104" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q104" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>